<commit_message>
fixed download, added add and edit functions
</commit_message>
<xml_diff>
--- a/upload/CreateTaxoList.xlsx
+++ b/upload/CreateTaxoList.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Python Messing Around/TTD API/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F24A04EB-F5F5-5F4D-BF19-AA5C769CBA0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FABBFF05-98D4-7942-8FBA-58E444020BF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateTaxoList" sheetId="1" r:id="rId1"/>
@@ -25,17 +25,9 @@
     <t>Segment ID</t>
   </si>
   <si>
-    <t>Parent
-Segment ID</t>
-  </si>
-  <si>
     <t>Segment Name</t>
   </si>
   <si>
-    <t>Segment
-Description</t>
-  </si>
-  <si>
     <t>Buyable</t>
   </si>
   <si>
@@ -88,12 +80,18 @@
   </si>
   <si>
     <t>Media &gt; TV And Film &gt; TV Channels Watched Live (Last 30 Days) &gt; Good Food</t>
+  </si>
+  <si>
+    <t>Parent Segment ID</t>
+  </si>
+  <si>
+    <t>Segment Description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
@@ -934,10 +932,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -946,51 +946,51 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1001,13 +1001,13 @@
         <v>4427</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -1016,7 +1016,7 @@
         <v>1.5</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1027,13 +1027,13 @@
         <v>7807</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -1042,7 +1042,7 @@
         <v>1.8</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1053,10 +1053,10 @@
         <v>32039</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -1065,7 +1065,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1076,13 +1076,13 @@
         <v>32048</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -1091,7 +1091,7 @@
         <v>1.2</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed message when loading
</commit_message>
<xml_diff>
--- a/upload/CreateTaxoList.xlsx
+++ b/upload/CreateTaxoList.xlsx
@@ -5,22 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Python Messing Around/TTD API/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FABBFF05-98D4-7942-8FBA-58E444020BF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5978E0-E4F1-F344-AA0E-902E6BD46B34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37800" yWindow="2480" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CreateTaxoList" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="AppNexus" sheetId="3" r:id="rId2"/>
+    <sheet name="TTD" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
   <si>
     <t>Segment ID</t>
   </si>
@@ -86,16 +88,65 @@
   </si>
   <si>
     <t>Segment Description</t>
+  </si>
+  <si>
+    <t>Segment id</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>short_name</t>
+  </si>
+  <si>
+    <t>segment price</t>
+  </si>
+  <si>
+    <t>expire_minutes</t>
+  </si>
+  <si>
+    <t>member_id</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>Is Public</t>
+  </si>
+  <si>
+    <t>Data Category ID</t>
+  </si>
+  <si>
+    <t>Global Bombora - Custom - PrimaryTarget_1.Xaxis.BK.BlackRock.GI.N.LB.JRD</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>Global Bombora - Custom - PrimaryTarget_2.Xaxis.BK.BlackRock.GI.N.LB.JRD</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>optional</t>
+  </si>
+  <si>
+    <t>Member Buyer ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -230,8 +281,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -411,8 +468,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -527,6 +596,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -572,12 +671,27 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -932,11 +1046,162 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05563D56-CBDE-B54E-B088-A7AD6DDC136B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2DFE33-156C-FF4B-85F5-5A363A8440C2}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4">
+        <v>-2147396174</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2.25</v>
+      </c>
+      <c r="E3" s="4">
+        <v>129600</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1706</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>4309</v>
+      </c>
+      <c r="J3" s="7">
+        <v>1661</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4">
+        <v>-2147396173</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="6">
+        <v>2.25</v>
+      </c>
+      <c r="E4" s="4">
+        <v>129600</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1706</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>4309</v>
+      </c>
+      <c r="J4" s="7">
+        <v>1661</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -968,19 +1233,19 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F2" t="s">

</xml_diff>

<commit_message>
get full path of ttd segments instead of just child name
</commit_message>
<xml_diff>
--- a/upload/CreateTaxoList.xlsx
+++ b/upload/CreateTaxoList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5978E0-E4F1-F344-AA0E-902E6BD46B34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFABBC6-54E1-3B4A-B7C7-94336B32ECD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37800" yWindow="2480" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1880" yWindow="7600" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>Segment ID</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Depth</t>
   </si>
   <si>
-    <t xml:space="preserve"> CPM/% of Media </t>
-  </si>
-  <si>
     <t>Segment Full Path</t>
   </si>
   <si>
@@ -96,46 +93,46 @@
     <t>code</t>
   </si>
   <si>
-    <t>short_name</t>
-  </si>
-  <si>
-    <t>segment price</t>
-  </si>
-  <si>
-    <t>expire_minutes</t>
-  </si>
-  <si>
-    <t>member_id</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
     <t>Is Public</t>
   </si>
   <si>
     <t>Data Category ID</t>
   </si>
   <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>optional</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Member ID</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Buyer Member Id</t>
+  </si>
+  <si>
     <t>Global Bombora - Custom - PrimaryTarget_1.Xaxis.BK.BlackRock.GI.N.LB.JRD</t>
   </si>
   <si>
-    <t>active</t>
-  </si>
-  <si>
     <t>Global Bombora - Custom - PrimaryTarget_2.Xaxis.BK.BlackRock.GI.N.LB.JRD</t>
   </si>
   <si>
-    <t>output</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>optional</t>
-  </si>
-  <si>
-    <t>Member Buyer ID</t>
+    <t>Global Bombora - Custom - PrimaryTarget_3.Xaxis.BK.BlackRock.GI.N.LB.JRD</t>
   </si>
 </sst>
 </file>
@@ -673,25 +670,23 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1059,135 +1054,164 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2DFE33-156C-FF4B-85F5-5A363A8440C2}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>37</v>
+      <c r="J1" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>36</v>
+      <c r="A2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3">
         <v>-2147396174</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="6">
+      <c r="C3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="11">
         <v>2.25</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>129600</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>1706</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="4" t="b">
+      <c r="G3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <v>4309</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3">
         <v>1661</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3">
         <v>-2147396173</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="6">
+      <c r="C4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="11">
         <v>2.25</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>129600</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>1706</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="4" t="b">
+      <c r="G4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>4309</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4">
+        <v>1661</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="3">
+        <v>-2147396172</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="11">
+        <v>2.25</v>
+      </c>
+      <c r="E5" s="3">
+        <v>129600</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1706</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>4309</v>
+      </c>
+      <c r="J5">
         <v>1661</v>
       </c>
     </row>
@@ -1201,61 +1225,61 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="E1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="H2" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1266,10 +1290,10 @@
         <v>4427</v>
       </c>
       <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -1277,11 +1301,11 @@
       <c r="F3">
         <v>3</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>1.5</v>
       </c>
       <c r="H3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1292,10 +1316,10 @@
         <v>7807</v>
       </c>
       <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
         <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
@@ -1303,11 +1327,11 @@
       <c r="F4">
         <v>3</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>1.8</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1318,10 +1342,10 @@
         <v>32039</v>
       </c>
       <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
         <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -1330,7 +1354,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1341,10 +1365,10 @@
         <v>32048</v>
       </c>
       <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
@@ -1352,11 +1376,11 @@
       <c r="F6">
         <v>4</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>1.2</v>
       </c>
       <c r="H6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>